<commit_message>
Corrected write column error
</commit_message>
<xml_diff>
--- a/Customer Call List - Cleaned2.xlsx
+++ b/Customer Call List - Cleaned2.xlsx
@@ -703,7 +703,7 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -729,7 +729,7 @@
       <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>67</v>
       </c>
     </row>
@@ -758,7 +758,7 @@
       <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -787,7 +787,7 @@
       <c r="H5" t="s">
         <v>28</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>69</v>
       </c>
     </row>
@@ -819,7 +819,7 @@
       <c r="I6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>70</v>
       </c>
     </row>
@@ -845,7 +845,7 @@
       <c r="H7" t="s">
         <v>36</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>71</v>
       </c>
     </row>
@@ -874,7 +874,7 @@
       <c r="H8" t="s">
         <v>40</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>72</v>
       </c>
     </row>
@@ -903,7 +903,7 @@
       <c r="H9" t="s">
         <v>43</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>73</v>
       </c>
     </row>
@@ -932,7 +932,7 @@
       <c r="H10" t="s">
         <v>47</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>74</v>
       </c>
     </row>
@@ -961,7 +961,7 @@
       <c r="H11" t="s">
         <v>50</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>75</v>
       </c>
     </row>
@@ -993,7 +993,7 @@
       <c r="I12" t="s">
         <v>56</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       <c r="H13" t="s">
         <v>59</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       <c r="I14" t="s">
         <v>64</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>